<commit_message>
removed column of status
</commit_message>
<xml_diff>
--- a/Project Tracker.xlsx
+++ b/Project Tracker.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -423,9 +423,6 @@
         <v>Notes</v>
       </c>
       <c r="G1" t="str">
-        <v>Status</v>
-      </c>
-      <c r="H1" t="str">
         <v>Commit Tag</v>
       </c>
     </row>
@@ -449,9 +446,6 @@
         <v>Initial planning and understanding requirements</v>
       </c>
       <c r="G2" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H2" t="str">
         <v>v0.0-planning</v>
       </c>
     </row>
@@ -475,9 +469,6 @@
         <v>Initialize backend with SQLAlchemy and proper folder organization</v>
       </c>
       <c r="G3" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H3" t="str">
         <v>v0.1-backend-init</v>
       </c>
     </row>
@@ -501,9 +492,6 @@
         <v>SQLAlchemy models with relationships and request/response schemas</v>
       </c>
       <c r="G4" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H4" t="str">
         <v>v0.2-db-models</v>
       </c>
     </row>
@@ -527,9 +515,6 @@
         <v>All REST endpoints for session and file management</v>
       </c>
       <c r="G5" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H5" t="str">
         <v>v0.3-api-crud</v>
       </c>
     </row>
@@ -553,9 +538,6 @@
         <v>Verify API functionality before building parsers</v>
       </c>
       <c r="G6" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H6" t="str">
         <v>v0.4-api-test</v>
       </c>
     </row>
@@ -579,9 +561,6 @@
         <v>Complete Traveler PDF parsing with table extraction</v>
       </c>
       <c r="G7" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H7" t="str">
         <v>v0.5-pdf-parser</v>
       </c>
     </row>
@@ -605,9 +584,6 @@
         <v>Image OCR with preprocessing pipeline for serial numbers</v>
       </c>
       <c r="G8" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H8" t="str">
         <v>v0.6-ocr</v>
       </c>
     </row>
@@ -631,9 +607,6 @@
         <v>Parse 1-4 Excel files and extract Job/Part/Revision</v>
       </c>
       <c r="G9" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H9" t="str">
         <v>v0.7-excel</v>
       </c>
     </row>
@@ -657,9 +630,6 @@
         <v>Normalize all data formats for accurate comparison</v>
       </c>
       <c r="G10" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H10" t="str">
         <v>v0.8-normalize</v>
       </c>
     </row>
@@ -683,9 +653,6 @@
         <v>Core validation logic with Pass/Warning/Fail/Info determination</v>
       </c>
       <c r="G11" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H11" t="str">
         <v>v0.9-validation</v>
       </c>
     </row>
@@ -709,9 +676,6 @@
         <v>Real-time progress updates during analysis</v>
       </c>
       <c r="G12" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H12" t="str">
         <v>v0.10-websocket</v>
       </c>
     </row>
@@ -735,9 +699,6 @@
         <v>Initialize frontend with Material-UI and routing</v>
       </c>
       <c r="G13" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H13" t="str">
         <v>v0.11-frontend-init</v>
       </c>
     </row>
@@ -761,9 +722,6 @@
         <v>Complete upload UI with react-dropzone</v>
       </c>
       <c r="G14" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H14" t="str">
         <v>v0.12-upload-ui</v>
       </c>
     </row>
@@ -787,9 +745,6 @@
         <v>Real-time progress display during analysis</v>
       </c>
       <c r="G15" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H15" t="str">
         <v>v0.13-progress</v>
       </c>
     </row>
@@ -813,9 +768,6 @@
         <v>Main results display with expandable check details</v>
       </c>
       <c r="G16" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H16" t="str">
         <v>v0.14-results</v>
       </c>
     </row>
@@ -839,9 +791,6 @@
         <v>Browse past analysis sessions</v>
       </c>
       <c r="G17" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H17" t="str">
         <v>v0.15-history</v>
       </c>
     </row>
@@ -865,9 +814,6 @@
         <v>Smart CSV export with all validation data</v>
       </c>
       <c r="G18" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H18" t="str">
         <v>v0.16-export</v>
       </c>
     </row>
@@ -891,9 +837,6 @@
         <v>Complete integration and testing of full flow</v>
       </c>
       <c r="G19" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H19" t="str">
         <v>v0.17-integration</v>
       </c>
     </row>
@@ -917,9 +860,6 @@
         <v>Full Docker setup with one-command deployment</v>
       </c>
       <c r="G20" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H20" t="str">
         <v>v0.18-docker</v>
       </c>
     </row>
@@ -943,9 +883,6 @@
         <v>Comprehensive testing with provided sample files</v>
       </c>
       <c r="G21" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H21" t="str">
         <v>v0.19-testing</v>
       </c>
     </row>
@@ -969,9 +906,6 @@
         <v>Deploy to Render/Railway/AWS and verify</v>
       </c>
       <c r="G22" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H22" t="str">
         <v>v0.20-deploy</v>
       </c>
     </row>
@@ -995,9 +929,6 @@
         <v>Complete project documentation</v>
       </c>
       <c r="G23" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H23" t="str">
         <v>v0.21-docs</v>
       </c>
     </row>
@@ -1021,9 +952,6 @@
         <v>5-minute demo showing all features</v>
       </c>
       <c r="G24" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H24" t="str">
         <v>v0.22-demo</v>
       </c>
     </row>
@@ -1047,9 +975,6 @@
         <v>Final quality check and deliverable preparation</v>
       </c>
       <c r="G25" t="str">
-        <v>Not Started</v>
-      </c>
-      <c r="H25" t="str">
         <v>v0.23-final</v>
       </c>
     </row>
@@ -1067,15 +992,12 @@
         <v/>
       </c>
       <c r="G26" t="str">
-        <v>TOTAL ESTIMATED:</v>
-      </c>
-      <c r="H26" t="str">
         <v>113.5 hours</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H26"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G26"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
session creation, File uploading, websocket inetegration, validation result componentens created and displayed
</commit_message>
<xml_diff>
--- a/Project Tracker.xlsx
+++ b/Project Tracker.xlsx
@@ -624,7 +624,7 @@
         <v>4.5</v>
       </c>
       <c r="E10" t="str">
-        <v/>
+        <v>2hrs</v>
       </c>
       <c r="F10" t="str">
         <v>Normalize all data formats for accurate comparison</v>
@@ -647,7 +647,7 @@
         <v>10.5</v>
       </c>
       <c r="E11" t="str">
-        <v/>
+        <v>2 hrs</v>
       </c>
       <c r="F11" t="str">
         <v>Core validation logic with Pass/Warning/Fail/Info determination</v>
@@ -670,7 +670,7 @@
         <v>4</v>
       </c>
       <c r="E12" t="str">
-        <v/>
+        <v>1 hr</v>
       </c>
       <c r="F12" t="str">
         <v>Real-time progress updates during analysis</v>
@@ -693,7 +693,7 @@
         <v>3.5</v>
       </c>
       <c r="E13" t="str">
-        <v/>
+        <v>15 min</v>
       </c>
       <c r="F13" t="str">
         <v>Initialize frontend with Material-UI and routing</v>
@@ -716,7 +716,7 @@
         <v>6</v>
       </c>
       <c r="E14" t="str">
-        <v/>
+        <v>1hr</v>
       </c>
       <c r="F14" t="str">
         <v>Complete upload UI with react-dropzone</v>
@@ -739,7 +739,7 @@
         <v>4</v>
       </c>
       <c r="E15" t="str">
-        <v/>
+        <v>1hr</v>
       </c>
       <c r="F15" t="str">
         <v>Real-time progress display during analysis</v>
@@ -762,7 +762,7 @@
         <v>7.5</v>
       </c>
       <c r="E16" t="str">
-        <v/>
+        <v>2hr</v>
       </c>
       <c r="F16" t="str">
         <v>Main results display with expandable check details</v>
@@ -785,7 +785,7 @@
         <v>5</v>
       </c>
       <c r="E17" t="str">
-        <v/>
+        <v>1hr</v>
       </c>
       <c r="F17" t="str">
         <v>Browse past analysis sessions</v>
@@ -831,7 +831,7 @@
         <v>8</v>
       </c>
       <c r="E19" t="str">
-        <v/>
+        <v>1hr</v>
       </c>
       <c r="F19" t="str">
         <v>Complete integration and testing of full flow</v>
@@ -854,7 +854,7 @@
         <v>7.5</v>
       </c>
       <c r="E20" t="str">
-        <v/>
+        <v>2hr</v>
       </c>
       <c r="F20" t="str">
         <v>Full Docker setup with one-command deployment</v>

</xml_diff>